<commit_message>
updated BOM with reference designators.
</commit_message>
<xml_diff>
--- a/BOM/WWVB Shield BOM.xlsx
+++ b/BOM/WWVB Shield BOM.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$33</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="154">
   <si>
     <t>Description</t>
   </si>
@@ -117,12 +117,6 @@
     <t>http://www.onsemi.com/pub_link/Collateral/MMBF4391LT1-D.PDF</t>
   </si>
   <si>
-    <t>Unit Price (1)</t>
-  </si>
-  <si>
-    <t>Total Cost (1)</t>
-  </si>
-  <si>
     <t>BK-885CT-ND</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>Eric Born and Josh Friend</t>
   </si>
   <si>
-    <t>PCB</t>
-  </si>
-  <si>
     <t>ERJ-6ENF1000V</t>
   </si>
   <si>
@@ -393,7 +384,106 @@
     <t>PRT-10007</t>
   </si>
   <si>
-    <t>REVISION A00</t>
+    <t>RES 4.7K OHM 1/8W 1% 0805 SMD</t>
+  </si>
+  <si>
+    <t>P4.70KCCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF4701V</t>
+  </si>
+  <si>
+    <t>http://www.sparkfun.com/datasheets/Prototyping/Connectors/18688.pdf</t>
+  </si>
+  <si>
+    <t>REVISION A03</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>D1, D2</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>BAT1</t>
+  </si>
+  <si>
+    <t>R16, R17</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R3, R7</t>
+  </si>
+  <si>
+    <t>R4, R5, R6, R8, R9, R10, R11, R12, R13, R14, R15</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R18, R19</t>
+  </si>
+  <si>
+    <t>C10, C11</t>
+  </si>
+  <si>
+    <t>C4, C7</t>
+  </si>
+  <si>
+    <t>C8, C13, C15, C16</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C5, C6, C12, C14, C17</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>Unit Price (QTY1)</t>
+  </si>
+  <si>
+    <t>Total Cost (QTY 1)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>PCB - 2LYR</t>
   </si>
 </sst>
 </file>
@@ -488,7 +578,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -499,8 +589,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -572,8 +664,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="12">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -582,6 +681,8 @@
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -915,7 +1016,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -924,36 +1025,38 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="6"/>
-    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.6640625" style="2" customWidth="1"/>
-    <col min="9" max="11" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="75.33203125" style="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1">
@@ -982,10 +1085,10 @@
         <v>5</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>8</v>
@@ -1013,7 +1116,9 @@
       <c r="F7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="H7" s="11">
         <v>1</v>
       </c>
@@ -1048,7 +1153,9 @@
       <c r="F8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="28" t="s">
+        <v>128</v>
+      </c>
       <c r="H8" s="11">
         <v>1</v>
       </c>
@@ -1083,7 +1190,9 @@
       <c r="F9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="H9" s="11">
         <v>1</v>
       </c>
@@ -1118,7 +1227,9 @@
       <c r="F10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="11"/>
+      <c r="G10" s="28" t="s">
+        <v>129</v>
+      </c>
       <c r="H10" s="11">
         <v>1</v>
       </c>
@@ -1136,24 +1247,26 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>132</v>
+      </c>
       <c r="H11" s="11">
         <v>1</v>
       </c>
@@ -1166,64 +1279,68 @@
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="28" t="s">
+        <v>126</v>
+      </c>
       <c r="H12" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="14">
         <v>0.35</v>
       </c>
       <c r="J12" s="14">
         <f t="shared" si="0"/>
-        <v>0.35</v>
+        <v>0.7</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>133</v>
+      </c>
       <c r="H13" s="11">
         <v>2</v>
       </c>
@@ -1236,29 +1353,31 @@
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>127</v>
+      </c>
       <c r="H14" s="11">
         <v>1</v>
       </c>
@@ -1271,29 +1390,31 @@
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="E15" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="F15" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="29" t="s">
+        <v>134</v>
+      </c>
       <c r="H15" s="11">
         <v>1</v>
       </c>
@@ -1306,29 +1427,31 @@
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="11"/>
+        <v>58</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="H16" s="17">
         <v>2</v>
       </c>
@@ -1336,34 +1459,36 @@
         <v>0.22</v>
       </c>
       <c r="J16" s="14">
-        <f t="shared" ref="J16:J30" si="1">H16*I16</f>
+        <f t="shared" ref="J16:J31" si="1">H16*I16</f>
         <v>0.44</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="11"/>
+        <v>58</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>136</v>
+      </c>
       <c r="H17" s="17">
         <v>1</v>
       </c>
@@ -1376,29 +1501,31 @@
       </c>
       <c r="K17" s="11"/>
       <c r="L17" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="11"/>
+        <v>58</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>137</v>
+      </c>
       <c r="H18" s="17">
         <v>1</v>
       </c>
@@ -1411,29 +1538,31 @@
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="11"/>
+      <c r="G19" s="10" t="s">
+        <v>138</v>
+      </c>
       <c r="H19" s="17">
         <v>1</v>
       </c>
@@ -1445,28 +1574,32 @@
         <v>1.5</v>
       </c>
       <c r="K19" s="11"/>
-      <c r="L19" s="10"/>
+      <c r="L19" s="12" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>139</v>
+      </c>
       <c r="H20" s="11">
         <v>1</v>
       </c>
@@ -1479,29 +1612,31 @@
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>140</v>
+      </c>
       <c r="H21" s="11">
         <v>2</v>
       </c>
@@ -1514,29 +1649,31 @@
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>125</v>
+      </c>
       <c r="H22" s="11">
         <v>1</v>
       </c>
@@ -1549,134 +1686,142 @@
       </c>
       <c r="K22" s="11"/>
       <c r="L22" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="16" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>73</v>
+      <c r="E23" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>142</v>
+      </c>
       <c r="H23" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="J23" s="14">
         <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K23" s="11"/>
       <c r="L23" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>143</v>
+      </c>
       <c r="H24" s="11">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I24" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="J24" s="14">
         <f t="shared" si="1"/>
-        <v>0.77</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K24" s="11"/>
       <c r="L24" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="16" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>100</v>
+        <v>47</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>141</v>
+      </c>
       <c r="H25" s="11">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I25" s="14">
-        <v>4.3999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J25" s="14">
         <f t="shared" si="1"/>
-        <v>8.7999999999999995E-2</v>
+        <v>0.77</v>
       </c>
       <c r="K25" s="11"/>
-      <c r="L25" s="12" t="s">
-        <v>102</v>
+      <c r="L25" s="15" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="16" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>144</v>
+      </c>
       <c r="H26" s="11">
         <v>2</v>
       </c>
@@ -1689,151 +1834,202 @@
       </c>
       <c r="K26" s="11"/>
       <c r="L26" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" s="26" customFormat="1">
-      <c r="A27" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="H27" s="11">
+        <v>2</v>
+      </c>
+      <c r="I27" s="14">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="J27" s="14">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="26" customFormat="1">
+      <c r="A28" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22">
+      <c r="B28" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="H28" s="22">
         <v>4</v>
       </c>
-      <c r="I27" s="24">
+      <c r="I28" s="24">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="J27" s="24">
+      <c r="J28" s="24">
         <f t="shared" si="1"/>
         <v>0.11600000000000001</v>
       </c>
-      <c r="K27" s="22"/>
-      <c r="L27" s="25" t="s">
+      <c r="K28" s="22"/>
+      <c r="L28" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="26" customFormat="1">
+      <c r="A29" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" s="26" customFormat="1">
-      <c r="A28" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="22" t="s">
+      <c r="D29" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22">
+      <c r="E29" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" s="22">
         <v>8</v>
       </c>
-      <c r="I28" s="24">
+      <c r="I29" s="24">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="J28" s="24">
+      <c r="J29" s="24">
         <f t="shared" si="1"/>
         <v>0.30399999999999999</v>
       </c>
-      <c r="K28" s="22"/>
-      <c r="L28" s="25" t="s">
+      <c r="K29" s="22"/>
+      <c r="L29" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="16" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="B30" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11">
+      <c r="E30" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="H30" s="11">
         <v>1</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I30" s="14">
         <v>0.16500000000000001</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J30" s="14">
         <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
-      <c r="K29" s="11"/>
-      <c r="L29" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11">
+      <c r="K30" s="11"/>
+      <c r="L30" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H31" s="11">
         <v>1</v>
       </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14">
+      <c r="I31" s="14"/>
+      <c r="J31" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K30" s="11"/>
-      <c r="L30" s="10"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="10"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="I32" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J32" s="3">
-        <f>SUM(J7:J30)</f>
-        <v>12.420999999999998</v>
-      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
     </row>
     <row r="33" spans="9:10">
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="J33" s="3">
+        <f>SUM(J7:J31)</f>
+        <v>12.840999999999999</v>
+      </c>
     </row>
     <row r="34" spans="9:10">
       <c r="I34" s="3"/>
@@ -2022,6 +2218,10 @@
     <row r="80" spans="9:10">
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="9:10">
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2046,24 +2246,24 @@
     <hyperlink ref="L15" r:id="rId18"/>
     <hyperlink ref="L20" r:id="rId19"/>
     <hyperlink ref="L21" r:id="rId20"/>
-    <hyperlink ref="L24" r:id="rId21"/>
-    <hyperlink ref="L23" r:id="rId22"/>
+    <hyperlink ref="L25" r:id="rId21"/>
+    <hyperlink ref="L24" r:id="rId22"/>
     <hyperlink ref="L22" r:id="rId23"/>
-    <hyperlink ref="E24" r:id="rId24" display="http://search.digikey.com/us/en/products/ERJ-6ENF4702V/P47.0KCCT-ND/1746873"/>
-    <hyperlink ref="E23" r:id="rId25" display="http://search.digikey.com/us/en/products/ERJ-6ENF1002V/P10.0KCCT-ND/119248"/>
+    <hyperlink ref="E25" r:id="rId24" display="http://search.digikey.com/us/en/products/ERJ-6ENF4702V/P47.0KCCT-ND/1746873"/>
+    <hyperlink ref="E24" r:id="rId25" display="http://search.digikey.com/us/en/products/ERJ-6ENF1002V/P10.0KCCT-ND/119248"/>
     <hyperlink ref="E22" r:id="rId26" display="http://search.digikey.com/us/en/products/ERJ-6ENF1001V/P1.00KCCT-ND/118957"/>
     <hyperlink ref="E21" r:id="rId27" display="http://search.digikey.com/us/en/products/ERJ-6ENF2200V/P220CCT-ND/1746831"/>
     <hyperlink ref="E20" r:id="rId28" display="http://search.digikey.com/us/en/products/ERJ-6ENF1000V/P100CCT-ND/118668"/>
-    <hyperlink ref="L29" r:id="rId29"/>
-    <hyperlink ref="E27" r:id="rId30"/>
-    <hyperlink ref="L27" r:id="rId31"/>
-    <hyperlink ref="E28" r:id="rId32"/>
-    <hyperlink ref="L28" r:id="rId33"/>
-    <hyperlink ref="E29" r:id="rId34"/>
-    <hyperlink ref="E25" r:id="rId35"/>
-    <hyperlink ref="L25" r:id="rId36"/>
-    <hyperlink ref="E26" r:id="rId37"/>
-    <hyperlink ref="L26" r:id="rId38"/>
+    <hyperlink ref="L30" r:id="rId29"/>
+    <hyperlink ref="E28" r:id="rId30"/>
+    <hyperlink ref="L28" r:id="rId31"/>
+    <hyperlink ref="E29" r:id="rId32"/>
+    <hyperlink ref="L29" r:id="rId33"/>
+    <hyperlink ref="E30" r:id="rId34"/>
+    <hyperlink ref="E26" r:id="rId35"/>
+    <hyperlink ref="L26" r:id="rId36"/>
+    <hyperlink ref="E27" r:id="rId37"/>
+    <hyperlink ref="L27" r:id="rId38"/>
     <hyperlink ref="E16" r:id="rId39"/>
     <hyperlink ref="L16" r:id="rId40"/>
     <hyperlink ref="E18" r:id="rId41"/>
@@ -2071,11 +2271,13 @@
     <hyperlink ref="E17" r:id="rId43"/>
     <hyperlink ref="L17" r:id="rId44"/>
     <hyperlink ref="E19" r:id="rId45"/>
+    <hyperlink ref="E23" r:id="rId46"/>
+    <hyperlink ref="L23" r:id="rId47"/>
+    <hyperlink ref="L19" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="49" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="F28:F29 F20:F24 F25:F26" numberStoredAsText="1"/>
+    <ignoredError sqref="F28:F30 F23:F27 F20:F22" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Updated BOM to include pricing with and without our radio and CMAX radio
</commit_message>
<xml_diff>
--- a/BOM/WWVB Shield BOM.xlsx
+++ b/BOM/WWVB Shield BOM.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24800" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24860" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="With Radio" sheetId="1" r:id="rId1"/>
+    <sheet name="CMAX" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'With Radio'!$A$1:$L$33</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="155">
   <si>
     <t>Description</t>
   </si>
@@ -484,6 +485,9 @@
   </si>
   <si>
     <t>PCB - 2LYR</t>
+  </si>
+  <si>
+    <t>CMAX WWVB Reciever</t>
   </si>
 </sst>
 </file>
@@ -578,10 +582,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -672,7 +678,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="14">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -683,6 +689,8 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1018,8 +1026,8 @@
   </sheetPr>
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2285,4 +2293,1057 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1.04</v>
+      </c>
+      <c r="J2" s="14">
+        <f t="shared" ref="J2:J7" si="0">H2*I2</f>
+        <v>1.04</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14">
+        <v>1.38</v>
+      </c>
+      <c r="J3" s="14">
+        <f t="shared" si="0"/>
+        <v>1.38</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1.66</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="0"/>
+        <v>1.66</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.48</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J8" s="14">
+        <f>H8*I8</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" s="11">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1.01</v>
+      </c>
+      <c r="J9" s="14">
+        <f>H9*I9</f>
+        <v>1.01</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" s="11">
+        <v>1</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="J10" s="14">
+        <f>H10*I10</f>
+        <v>0.35</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="17">
+        <v>2</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" ref="J11:J26" si="1">H11*I11</f>
+        <v>0.44</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" s="17">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0.41</v>
+      </c>
+      <c r="J12" s="14">
+        <f t="shared" si="1"/>
+        <v>0.41</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="17">
+        <v>1</v>
+      </c>
+      <c r="I13" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="J13" s="14">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" s="17">
+        <v>1</v>
+      </c>
+      <c r="I14" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="J14" s="14">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J15" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J17" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J18" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="11">
+        <v>0</v>
+      </c>
+      <c r="I19" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J20" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="11">
+        <v>0</v>
+      </c>
+      <c r="I21" s="14">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="11">
+        <v>0</v>
+      </c>
+      <c r="I22" s="14">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23" s="22">
+        <v>4</v>
+      </c>
+      <c r="I23" s="24">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="J23" s="24">
+        <f t="shared" si="1"/>
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="K23" s="22"/>
+      <c r="L23" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="22">
+        <v>8</v>
+      </c>
+      <c r="I24" s="24">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J24" s="24">
+        <f t="shared" si="1"/>
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="K24" s="22"/>
+      <c r="L24" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="H25" s="11">
+        <v>0</v>
+      </c>
+      <c r="I25" s="14">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="J25" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H26" s="11">
+        <v>1</v>
+      </c>
+      <c r="I26" s="14">
+        <v>11</v>
+      </c>
+      <c r="J26" s="14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="I28" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" s="3">
+        <f>SUM(J2:J26)</f>
+        <v>20.939999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E7" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="L2" r:id="rId10"/>
+    <hyperlink ref="L3" r:id="rId11"/>
+    <hyperlink ref="L4" r:id="rId12"/>
+    <hyperlink ref="L5" r:id="rId13"/>
+    <hyperlink ref="L6" r:id="rId14"/>
+    <hyperlink ref="L7" r:id="rId15"/>
+    <hyperlink ref="L8" r:id="rId16"/>
+    <hyperlink ref="L9" r:id="rId17"/>
+    <hyperlink ref="L10" r:id="rId18"/>
+    <hyperlink ref="L15" r:id="rId19"/>
+    <hyperlink ref="L16" r:id="rId20"/>
+    <hyperlink ref="L20" r:id="rId21"/>
+    <hyperlink ref="L19" r:id="rId22"/>
+    <hyperlink ref="L17" r:id="rId23"/>
+    <hyperlink ref="E20" r:id="rId24" display="http://search.digikey.com/us/en/products/ERJ-6ENF4702V/P47.0KCCT-ND/1746873"/>
+    <hyperlink ref="E19" r:id="rId25" display="http://search.digikey.com/us/en/products/ERJ-6ENF1002V/P10.0KCCT-ND/119248"/>
+    <hyperlink ref="E17" r:id="rId26" display="http://search.digikey.com/us/en/products/ERJ-6ENF1001V/P1.00KCCT-ND/118957"/>
+    <hyperlink ref="E16" r:id="rId27" display="http://search.digikey.com/us/en/products/ERJ-6ENF2200V/P220CCT-ND/1746831"/>
+    <hyperlink ref="E15" r:id="rId28" display="http://search.digikey.com/us/en/products/ERJ-6ENF1000V/P100CCT-ND/118668"/>
+    <hyperlink ref="L25" r:id="rId29"/>
+    <hyperlink ref="E23" r:id="rId30"/>
+    <hyperlink ref="L23" r:id="rId31"/>
+    <hyperlink ref="E24" r:id="rId32"/>
+    <hyperlink ref="L24" r:id="rId33"/>
+    <hyperlink ref="E25" r:id="rId34"/>
+    <hyperlink ref="E21" r:id="rId35"/>
+    <hyperlink ref="L21" r:id="rId36"/>
+    <hyperlink ref="E22" r:id="rId37"/>
+    <hyperlink ref="L22" r:id="rId38"/>
+    <hyperlink ref="E11" r:id="rId39"/>
+    <hyperlink ref="L11" r:id="rId40"/>
+    <hyperlink ref="E13" r:id="rId41"/>
+    <hyperlink ref="L13" r:id="rId42"/>
+    <hyperlink ref="E12" r:id="rId43"/>
+    <hyperlink ref="L12" r:id="rId44"/>
+    <hyperlink ref="E14" r:id="rId45"/>
+    <hyperlink ref="E18" r:id="rId46"/>
+    <hyperlink ref="L18" r:id="rId47"/>
+    <hyperlink ref="L14" r:id="rId48"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>